<commit_message>
One time email feature added
</commit_message>
<xml_diff>
--- a/Clients.xlsx
+++ b/Clients.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\OneDrive - ualberta.ca\Desktop\Career\Email Automation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\OneDrive - ualberta.ca\Desktop\Career\Independent Projects\Email Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECA677EB-9EE4-4A8D-B54F-62A80A7A0113}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7FF4F4D-18E7-48F5-9731-83040F7EACFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4500" yWindow="4185" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -463,7 +463,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -559,8 +559,8 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{D96C61BC-96F1-4C6C-B8D9-427D4B356025}"/>
-    <hyperlink ref="A3:A4" r:id="rId2" display="abc@example.com" xr:uid="{1011B1A3-C338-4342-9CDA-26CB3B68DABB}"/>
+    <hyperlink ref="A3:A4" r:id="rId1" display="abc@example.com" xr:uid="{1011B1A3-C338-4342-9CDA-26CB3B68DABB}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{D96C61BC-96F1-4C6C-B8D9-427D4B356025}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>

</xml_diff>